<commit_message>
dataset 1 e 3 - completos
</commit_message>
<xml_diff>
--- a/StockingProblemProject/Testes/Problema3/testes_tamanho_populacao/statistic_average_fitness_avaliado.xlsx
+++ b/StockingProblemProject/Testes/Problema3/testes_tamanho_populacao/statistic_average_fitness_avaliado.xlsx
@@ -1,26 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\AppData\Local\GitHubDesktop\app-2.8.3\IAProject_StockingProblem\StockingProblemProject\Testes\Problema3\testes_tamanho_populacao\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bruna Leitão\Desktop\Escola\IA\IAProject_StockingProblem\StockingProblemProject\Testes\Problema3\testes_tamanho_populacao\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{B4E9EF60-49B3-4FFF-A316-064C94651420}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{DB0CA920-E97A-4699-9A12-93121A88D7D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-109" yWindow="-109" windowWidth="26301" windowHeight="14889"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12696" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="statistic_average_fitness_avali" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="23">
   <si>
     <t>Population size:</t>
   </si>
@@ -87,11 +98,14 @@
   <si>
     <t>Average/(Population * Generations)</t>
   </si>
+  <si>
+    <t>A melhor combinação em relação ao calculo de Average/(Popupation*Generations) é de pop 50 e ger 100. Mas a média aumenta de 339,48 para 348,06 por isso vamos optar pela combinação de pop 150 e ger 175</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -234,7 +248,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="35">
+  <fills count="36">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -426,6 +440,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -587,16 +607,20 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="3" fontId="0" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="3" fontId="0" fillId="35" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Cor1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -736,7 +760,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent6"/>
+                <a:schemeClr val="accent4"/>
               </a:solidFill>
               <a:ln>
                 <a:noFill/>
@@ -1183,7 +1207,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent6"/>
+                <a:schemeClr val="accent4"/>
               </a:solidFill>
               <a:ln>
                 <a:noFill/>
@@ -1529,6 +1553,498 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="pt-PT"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="pt-PT"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>statistic_average_fitness_avali!$O$47</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Average/(Population * Generations)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-C910-4F60-827C-9B667AC8AF59}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="13"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000002-C910-4F60-827C-9B667AC8AF59}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>statistic_average_fitness_avali!$L$48:$M$67</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="20"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>ger 100</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>ger 125</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>ger 150</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>ger 175</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>ger 100</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>ger 125</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>ger 100</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>ger 150</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>ger 175</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>ger 125</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>ger 100</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>ger 150</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>ger 125</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>ger 175</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>ger 150</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
+                    <c:v>ger 175</c:v>
+                  </c:pt>
+                  <c:pt idx="16">
+                    <c:v>ger 100</c:v>
+                  </c:pt>
+                  <c:pt idx="17">
+                    <c:v>ger 125</c:v>
+                  </c:pt>
+                  <c:pt idx="18">
+                    <c:v>ger 150</c:v>
+                  </c:pt>
+                  <c:pt idx="19">
+                    <c:v>ger 175</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>pop 50</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>pop 50</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>pop 50</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>pop 50</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>pop 100</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>pop 100</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>pop 150</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>pop 100</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>pop 100</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>pop 150</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>pop 200</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>pop 150</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>pop 200</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>pop 150</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>pop 200</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
+                    <c:v>pop 200</c:v>
+                  </c:pt>
+                  <c:pt idx="16">
+                    <c:v>pop 400</c:v>
+                  </c:pt>
+                  <c:pt idx="17">
+                    <c:v>pop 400</c:v>
+                  </c:pt>
+                  <c:pt idx="18">
+                    <c:v>pop 400</c:v>
+                  </c:pt>
+                  <c:pt idx="19">
+                    <c:v>pop 400</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>statistic_average_fitness_avali!$O$48:$O$67</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>6.9611999999999993E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.5536000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.6128000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.9430857E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.4493999999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.7409599999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.3081332999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.2733333000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.9439999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.8315733000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.7448999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.5170667000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.3854399999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.2932571E-2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.1454667E-2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>9.7634290000000006E-3</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>8.8454999999999992E-3</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>7.0331999999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>5.830333E-3</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>4.9645710000000001E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-C910-4F60-827C-9B667AC8AF59}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="599971256"/>
+        <c:axId val="599971896"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="599971256"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-PT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="599971896"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="599971896"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-PT"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="599971256"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pt-PT"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1609,6 +2125,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -2585,6 +3141,509 @@
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -2686,6 +3745,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>99060</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>64770</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>579120</xdr:colOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>106680</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Gráfico 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5A5C52B7-8ECD-4C20-86CD-04343BCB192D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2990,19 +4085,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N43"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:P74"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
+    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
+      <selection activeCell="R77" sqref="R77"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="11" max="11" width="1.375" style="2" customWidth="1"/>
+    <col min="11" max="11" width="1.33203125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3040,7 +4135,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>50</v>
       </c>
@@ -3068,7 +4163,7 @@
       <c r="J2" s="1">
         <v>5077046385448920</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="L2" s="5" t="s">
         <v>12</v>
       </c>
       <c r="M2" t="s">
@@ -3078,7 +4173,7 @@
         <v>348.06</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>50</v>
       </c>
@@ -3106,7 +4201,7 @@
       <c r="J3" s="1">
         <v>5044799302251770</v>
       </c>
-      <c r="L3" s="3"/>
+      <c r="L3" s="5"/>
       <c r="M3" t="s">
         <v>14</v>
       </c>
@@ -3114,7 +4209,7 @@
         <v>347.1</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>50</v>
       </c>
@@ -3142,7 +4237,7 @@
       <c r="J4" s="1">
         <v>4745355624186660</v>
       </c>
-      <c r="L4" s="3"/>
+      <c r="L4" s="5"/>
       <c r="M4" t="s">
         <v>15</v>
       </c>
@@ -3150,7 +4245,7 @@
         <v>345.96</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>50</v>
       </c>
@@ -3178,7 +4273,7 @@
       <c r="J5" s="1">
         <v>4789530248364650</v>
       </c>
-      <c r="L5" s="3"/>
+      <c r="L5" s="5"/>
       <c r="M5" t="s">
         <v>16</v>
       </c>
@@ -3186,7 +4281,7 @@
         <v>345.02</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>100</v>
       </c>
@@ -3214,7 +4309,7 @@
       <c r="J6" s="1">
         <v>5576414618731280</v>
       </c>
-      <c r="L6" s="3" t="s">
+      <c r="L6" s="5" t="s">
         <v>17</v>
       </c>
       <c r="M6" t="s">
@@ -3224,7 +4319,7 @@
         <v>344.94</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>100</v>
       </c>
@@ -3252,7 +4347,7 @@
       <c r="J7" s="1">
         <v>5440183820423710</v>
       </c>
-      <c r="L7" s="3"/>
+      <c r="L7" s="5"/>
       <c r="M7" t="s">
         <v>14</v>
       </c>
@@ -3260,7 +4355,7 @@
         <v>342.62</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>100</v>
       </c>
@@ -3288,7 +4383,7 @@
       <c r="J8" s="1">
         <v>5649778756730210</v>
       </c>
-      <c r="L8" s="3"/>
+      <c r="L8" s="5"/>
       <c r="M8" t="s">
         <v>15</v>
       </c>
@@ -3296,7 +4391,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>100</v>
       </c>
@@ -3324,7 +4419,7 @@
       <c r="J9" s="1">
         <v>596657355607052</v>
       </c>
-      <c r="L9" s="3"/>
+      <c r="L9" s="5"/>
       <c r="M9" t="s">
         <v>16</v>
       </c>
@@ -3332,7 +4427,7 @@
         <v>340.2</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>150</v>
       </c>
@@ -3360,7 +4455,7 @@
       <c r="J10" s="1">
         <v>6242723764511760</v>
       </c>
-      <c r="L10" s="3" t="s">
+      <c r="L10" s="5" t="s">
         <v>18</v>
       </c>
       <c r="M10" t="s">
@@ -3370,7 +4465,7 @@
         <v>346.22</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>150</v>
       </c>
@@ -3398,7 +4493,7 @@
       <c r="J11" s="1">
         <v>6847159995209690</v>
       </c>
-      <c r="L11" s="3"/>
+      <c r="L11" s="5"/>
       <c r="M11" t="s">
         <v>14</v>
       </c>
@@ -3406,7 +4501,7 @@
         <v>343.42</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>150</v>
       </c>
@@ -3434,7 +4529,7 @@
       <c r="J12" s="1">
         <v>6958764258113650</v>
       </c>
-      <c r="L12" s="3"/>
+      <c r="L12" s="5"/>
       <c r="M12" t="s">
         <v>15</v>
       </c>
@@ -3442,7 +4537,7 @@
         <v>341.34</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>150</v>
       </c>
@@ -3470,7 +4565,7 @@
       <c r="J13" s="1">
         <v>6576442807475780</v>
       </c>
-      <c r="L13" s="3"/>
+      <c r="L13" s="5"/>
       <c r="M13" t="s">
         <v>16</v>
       </c>
@@ -3478,7 +4573,7 @@
         <v>339.48</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>200</v>
       </c>
@@ -3506,7 +4601,7 @@
       <c r="J14" s="1">
         <v>6392151437505210</v>
       </c>
-      <c r="L14" s="3" t="s">
+      <c r="L14" s="5" t="s">
         <v>19</v>
       </c>
       <c r="M14" t="s">
@@ -3516,7 +4611,7 @@
         <v>348.98</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>200</v>
       </c>
@@ -3544,7 +4639,7 @@
       <c r="J15" s="1">
         <v>6854954412685760</v>
       </c>
-      <c r="L15" s="3"/>
+      <c r="L15" s="5"/>
       <c r="M15" t="s">
         <v>14</v>
       </c>
@@ -3552,7 +4647,7 @@
         <v>346.36</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>200</v>
       </c>
@@ -3580,7 +4675,7 @@
       <c r="J16" s="1">
         <v>6819853370857760</v>
       </c>
-      <c r="L16" s="3"/>
+      <c r="L16" s="5"/>
       <c r="M16" t="s">
         <v>15</v>
       </c>
@@ -3588,7 +4683,7 @@
         <v>343.64</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>200</v>
       </c>
@@ -3616,7 +4711,7 @@
       <c r="J17" s="1">
         <v>647468918172911</v>
       </c>
-      <c r="L17" s="3"/>
+      <c r="L17" s="5"/>
       <c r="M17" t="s">
         <v>16</v>
       </c>
@@ -3624,7 +4719,7 @@
         <v>341.72</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>400</v>
       </c>
@@ -3652,7 +4747,7 @@
       <c r="J18" s="1">
         <v>455495334773036</v>
       </c>
-      <c r="L18" s="3" t="s">
+      <c r="L18" s="5" t="s">
         <v>20</v>
       </c>
       <c r="M18" t="s">
@@ -3662,7 +4757,7 @@
         <v>353.82</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>400</v>
       </c>
@@ -3690,7 +4785,7 @@
       <c r="J19" s="1">
         <v>5870638806807990</v>
       </c>
-      <c r="L19" s="3"/>
+      <c r="L19" s="5"/>
       <c r="M19" t="s">
         <v>14</v>
       </c>
@@ -3698,7 +4793,7 @@
         <v>351.66</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>400</v>
       </c>
@@ -3726,7 +4821,7 @@
       <c r="J20" s="1">
         <v>6348826663250460</v>
       </c>
-      <c r="L20" s="3"/>
+      <c r="L20" s="5"/>
       <c r="M20" t="s">
         <v>15</v>
       </c>
@@ -3734,7 +4829,7 @@
         <v>349.82</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>400</v>
       </c>
@@ -3762,7 +4857,7 @@
       <c r="J21" s="1">
         <v>6735695955133360</v>
       </c>
-      <c r="L21" s="3"/>
+      <c r="L21" s="5"/>
       <c r="M21" t="s">
         <v>16</v>
       </c>
@@ -3770,8 +4865,8 @@
         <v>347.52</v>
       </c>
     </row>
-    <row r="22" spans="1:14" s="2" customFormat="1" ht="8.15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="23" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" s="2" customFormat="1" ht="8.1" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="23" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>0</v>
       </c>
@@ -3811,36 +4906,36 @@
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A24" s="5">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A24" s="6">
         <v>150</v>
       </c>
-      <c r="B24" s="5">
+      <c r="B24" s="6">
         <v>175</v>
       </c>
-      <c r="C24" s="5" t="s">
+      <c r="C24" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="D24" s="5" t="s">
+      <c r="D24" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="E24" s="5">
+      <c r="E24" s="6">
         <v>0.6</v>
       </c>
-      <c r="F24" s="5" t="s">
+      <c r="F24" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="G24" s="5">
+      <c r="G24" s="6">
         <v>0.4</v>
       </c>
-      <c r="H24" s="5"/>
-      <c r="I24" s="5">
+      <c r="H24" s="6"/>
+      <c r="I24" s="6">
         <v>339.48</v>
       </c>
-      <c r="J24" s="6">
+      <c r="J24" s="7">
         <v>6576442807475780</v>
       </c>
-      <c r="L24" s="3" t="s">
+      <c r="L24" s="5" t="s">
         <v>12</v>
       </c>
       <c r="M24" t="s">
@@ -3851,7 +4946,7 @@
         <v>6.9612000000000007E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>100</v>
       </c>
@@ -3879,7 +4974,7 @@
       <c r="J25" s="1">
         <v>596657355607052</v>
       </c>
-      <c r="L25" s="3"/>
+      <c r="L25" s="5"/>
       <c r="M25" t="s">
         <v>14</v>
       </c>
@@ -3888,7 +4983,7 @@
         <v>5.5536000000000002E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>100</v>
       </c>
@@ -3916,7 +5011,7 @@
       <c r="J26" s="1">
         <v>5649778756730210</v>
       </c>
-      <c r="L26" s="3"/>
+      <c r="L26" s="5"/>
       <c r="M26" t="s">
         <v>15</v>
       </c>
@@ -3925,7 +5020,7 @@
         <v>4.6127999999999995E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>150</v>
       </c>
@@ -3953,7 +5048,7 @@
       <c r="J27" s="1">
         <v>6958764258113650</v>
       </c>
-      <c r="L27" s="3"/>
+      <c r="L27" s="5"/>
       <c r="M27" t="s">
         <v>16</v>
       </c>
@@ -3962,7 +5057,7 @@
         <v>3.9430857142857142E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>200</v>
       </c>
@@ -3990,7 +5085,7 @@
       <c r="J28" s="1">
         <v>647468918172911</v>
       </c>
-      <c r="L28" s="3" t="s">
+      <c r="L28" s="5" t="s">
         <v>17</v>
       </c>
       <c r="M28" t="s">
@@ -4001,7 +5096,7 @@
         <v>3.4493999999999997E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>100</v>
       </c>
@@ -4029,7 +5124,7 @@
       <c r="J29" s="1">
         <v>5440183820423710</v>
       </c>
-      <c r="L29" s="3"/>
+      <c r="L29" s="5"/>
       <c r="M29" t="s">
         <v>14</v>
       </c>
@@ -4038,7 +5133,7 @@
         <v>2.7409599999999999E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>150</v>
       </c>
@@ -4066,7 +5161,7 @@
       <c r="J30" s="1">
         <v>6847159995209690</v>
       </c>
-      <c r="L30" s="3"/>
+      <c r="L30" s="5"/>
       <c r="M30" t="s">
         <v>15</v>
       </c>
@@ -4075,7 +5170,7 @@
         <v>2.2733333333333335E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>200</v>
       </c>
@@ -4103,7 +5198,7 @@
       <c r="J31" s="1">
         <v>6819853370857760</v>
       </c>
-      <c r="L31" s="3"/>
+      <c r="L31" s="5"/>
       <c r="M31" t="s">
         <v>16</v>
       </c>
@@ -4112,7 +5207,7 @@
         <v>1.9439999999999999E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>100</v>
       </c>
@@ -4140,7 +5235,7 @@
       <c r="J32" s="1">
         <v>5576414618731280</v>
       </c>
-      <c r="L32" s="3" t="s">
+      <c r="L32" s="5" t="s">
         <v>18</v>
       </c>
       <c r="M32" t="s">
@@ -4151,7 +5246,7 @@
         <v>2.3081333333333336E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>50</v>
       </c>
@@ -4179,7 +5274,7 @@
       <c r="J33" s="1">
         <v>4789530248364650</v>
       </c>
-      <c r="L33" s="3"/>
+      <c r="L33" s="5"/>
       <c r="M33" t="s">
         <v>14</v>
       </c>
@@ -4188,7 +5283,7 @@
         <v>1.8315733333333334E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>50</v>
       </c>
@@ -4216,7 +5311,7 @@
       <c r="J34" s="1">
         <v>4745355624186660</v>
       </c>
-      <c r="L34" s="3"/>
+      <c r="L34" s="5"/>
       <c r="M34" t="s">
         <v>15</v>
       </c>
@@ -4225,7 +5320,7 @@
         <v>1.5170666666666666E-2</v>
       </c>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>150</v>
       </c>
@@ -4253,7 +5348,7 @@
       <c r="J35" s="1">
         <v>6242723764511760</v>
       </c>
-      <c r="L35" s="3"/>
+      <c r="L35" s="5"/>
       <c r="M35" t="s">
         <v>16</v>
       </c>
@@ -4262,7 +5357,7 @@
         <v>1.2932571428571429E-2</v>
       </c>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>200</v>
       </c>
@@ -4290,7 +5385,7 @@
       <c r="J36" s="1">
         <v>6854954412685760</v>
       </c>
-      <c r="L36" s="3" t="s">
+      <c r="L36" s="5" t="s">
         <v>19</v>
       </c>
       <c r="M36" t="s">
@@ -4301,7 +5396,7 @@
         <v>1.7448999999999999E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>50</v>
       </c>
@@ -4329,7 +5424,7 @@
       <c r="J37" s="1">
         <v>5044799302251770</v>
       </c>
-      <c r="L37" s="3"/>
+      <c r="L37" s="5"/>
       <c r="M37" t="s">
         <v>14</v>
       </c>
@@ -4338,7 +5433,7 @@
         <v>1.3854400000000001E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>400</v>
       </c>
@@ -4366,7 +5461,7 @@
       <c r="J38" s="1">
         <v>6735695955133360</v>
       </c>
-      <c r="L38" s="3"/>
+      <c r="L38" s="5"/>
       <c r="M38" t="s">
         <v>15</v>
       </c>
@@ -4375,7 +5470,7 @@
         <v>1.1454666666666667E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>50</v>
       </c>
@@ -4403,7 +5498,7 @@
       <c r="J39" s="1">
         <v>5077046385448920</v>
       </c>
-      <c r="L39" s="3"/>
+      <c r="L39" s="5"/>
       <c r="M39" t="s">
         <v>16</v>
       </c>
@@ -4412,7 +5507,7 @@
         <v>9.7634285714285722E-3</v>
       </c>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>200</v>
       </c>
@@ -4440,7 +5535,7 @@
       <c r="J40" s="1">
         <v>6392151437505210</v>
       </c>
-      <c r="L40" s="3" t="s">
+      <c r="L40" s="5" t="s">
         <v>20</v>
       </c>
       <c r="M40" t="s">
@@ -4451,7 +5546,7 @@
         <v>8.8454999999999992E-3</v>
       </c>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>400</v>
       </c>
@@ -4479,7 +5574,7 @@
       <c r="J41" s="1">
         <v>6348826663250460</v>
       </c>
-      <c r="L41" s="3"/>
+      <c r="L41" s="5"/>
       <c r="M41" t="s">
         <v>14</v>
       </c>
@@ -4488,7 +5583,7 @@
         <v>7.0332000000000007E-3</v>
       </c>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>400</v>
       </c>
@@ -4516,7 +5611,7 @@
       <c r="J42" s="1">
         <v>5870638806807990</v>
       </c>
-      <c r="L42" s="3"/>
+      <c r="L42" s="5"/>
       <c r="M42" t="s">
         <v>15</v>
       </c>
@@ -4525,7 +5620,7 @@
         <v>5.8303333333333332E-3</v>
       </c>
     </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>400</v>
       </c>
@@ -4553,7 +5648,7 @@
       <c r="J43" s="1">
         <v>455495334773036</v>
       </c>
-      <c r="L43" s="3"/>
+      <c r="L43" s="5"/>
       <c r="M43" t="s">
         <v>16</v>
       </c>
@@ -4562,11 +5657,350 @@
         <v>4.9645714285714284E-3</v>
       </c>
     </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="L47" t="s">
+        <v>0</v>
+      </c>
+      <c r="M47" t="s">
+        <v>1</v>
+      </c>
+      <c r="N47" t="s">
+        <v>7</v>
+      </c>
+      <c r="O47" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="L48" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="M48" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="N48" s="4">
+        <v>348.06</v>
+      </c>
+      <c r="O48" s="4">
+        <v>6.9611999999999993E-2</v>
+      </c>
+    </row>
+    <row r="49" spans="12:15" x14ac:dyDescent="0.3">
+      <c r="L49" t="s">
+        <v>12</v>
+      </c>
+      <c r="M49" t="s">
+        <v>14</v>
+      </c>
+      <c r="N49">
+        <v>347.1</v>
+      </c>
+      <c r="O49">
+        <v>5.5536000000000002E-2</v>
+      </c>
+    </row>
+    <row r="50" spans="12:15" x14ac:dyDescent="0.3">
+      <c r="L50" t="s">
+        <v>12</v>
+      </c>
+      <c r="M50" t="s">
+        <v>15</v>
+      </c>
+      <c r="N50">
+        <v>345.96</v>
+      </c>
+      <c r="O50">
+        <v>4.6128000000000002E-2</v>
+      </c>
+    </row>
+    <row r="51" spans="12:15" x14ac:dyDescent="0.3">
+      <c r="L51" t="s">
+        <v>12</v>
+      </c>
+      <c r="M51" t="s">
+        <v>16</v>
+      </c>
+      <c r="N51">
+        <v>345.02</v>
+      </c>
+      <c r="O51">
+        <v>3.9430857E-2</v>
+      </c>
+    </row>
+    <row r="52" spans="12:15" x14ac:dyDescent="0.3">
+      <c r="L52" t="s">
+        <v>17</v>
+      </c>
+      <c r="M52" t="s">
+        <v>13</v>
+      </c>
+      <c r="N52">
+        <v>344.94</v>
+      </c>
+      <c r="O52">
+        <v>3.4493999999999997E-2</v>
+      </c>
+    </row>
+    <row r="53" spans="12:15" x14ac:dyDescent="0.3">
+      <c r="L53" t="s">
+        <v>17</v>
+      </c>
+      <c r="M53" t="s">
+        <v>14</v>
+      </c>
+      <c r="N53">
+        <v>342.62</v>
+      </c>
+      <c r="O53">
+        <v>2.7409599999999999E-2</v>
+      </c>
+    </row>
+    <row r="54" spans="12:15" x14ac:dyDescent="0.3">
+      <c r="L54" t="s">
+        <v>18</v>
+      </c>
+      <c r="M54" t="s">
+        <v>13</v>
+      </c>
+      <c r="N54">
+        <v>346.22</v>
+      </c>
+      <c r="O54">
+        <v>2.3081332999999999E-2</v>
+      </c>
+    </row>
+    <row r="55" spans="12:15" x14ac:dyDescent="0.3">
+      <c r="L55" t="s">
+        <v>17</v>
+      </c>
+      <c r="M55" t="s">
+        <v>15</v>
+      </c>
+      <c r="N55">
+        <v>341</v>
+      </c>
+      <c r="O55">
+        <v>2.2733333000000001E-2</v>
+      </c>
+    </row>
+    <row r="56" spans="12:15" x14ac:dyDescent="0.3">
+      <c r="L56" t="s">
+        <v>17</v>
+      </c>
+      <c r="M56" t="s">
+        <v>16</v>
+      </c>
+      <c r="N56">
+        <v>340.2</v>
+      </c>
+      <c r="O56">
+        <v>1.9439999999999999E-2</v>
+      </c>
+    </row>
+    <row r="57" spans="12:15" x14ac:dyDescent="0.3">
+      <c r="L57" t="s">
+        <v>18</v>
+      </c>
+      <c r="M57" t="s">
+        <v>14</v>
+      </c>
+      <c r="N57">
+        <v>343.42</v>
+      </c>
+      <c r="O57">
+        <v>1.8315733000000001E-2</v>
+      </c>
+    </row>
+    <row r="58" spans="12:15" x14ac:dyDescent="0.3">
+      <c r="L58" t="s">
+        <v>19</v>
+      </c>
+      <c r="M58" t="s">
+        <v>13</v>
+      </c>
+      <c r="N58">
+        <v>348.98</v>
+      </c>
+      <c r="O58">
+        <v>1.7448999999999999E-2</v>
+      </c>
+    </row>
+    <row r="59" spans="12:15" x14ac:dyDescent="0.3">
+      <c r="L59" t="s">
+        <v>18</v>
+      </c>
+      <c r="M59" t="s">
+        <v>15</v>
+      </c>
+      <c r="N59">
+        <v>341.34</v>
+      </c>
+      <c r="O59">
+        <v>1.5170667000000001E-2</v>
+      </c>
+    </row>
+    <row r="60" spans="12:15" x14ac:dyDescent="0.3">
+      <c r="L60" t="s">
+        <v>19</v>
+      </c>
+      <c r="M60" t="s">
+        <v>14</v>
+      </c>
+      <c r="N60">
+        <v>346.36</v>
+      </c>
+      <c r="O60">
+        <v>1.3854399999999999E-2</v>
+      </c>
+    </row>
+    <row r="61" spans="12:15" x14ac:dyDescent="0.3">
+      <c r="L61" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="M61" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="N61" s="3">
+        <v>339.48</v>
+      </c>
+      <c r="O61">
+        <v>1.2932571E-2</v>
+      </c>
+    </row>
+    <row r="62" spans="12:15" x14ac:dyDescent="0.3">
+      <c r="L62" t="s">
+        <v>19</v>
+      </c>
+      <c r="M62" t="s">
+        <v>15</v>
+      </c>
+      <c r="N62">
+        <v>343.64</v>
+      </c>
+      <c r="O62">
+        <v>1.1454667E-2</v>
+      </c>
+    </row>
+    <row r="63" spans="12:15" x14ac:dyDescent="0.3">
+      <c r="L63" t="s">
+        <v>19</v>
+      </c>
+      <c r="M63" t="s">
+        <v>16</v>
+      </c>
+      <c r="N63">
+        <v>341.72</v>
+      </c>
+      <c r="O63">
+        <v>9.7634290000000006E-3</v>
+      </c>
+    </row>
+    <row r="64" spans="12:15" x14ac:dyDescent="0.3">
+      <c r="L64" t="s">
+        <v>20</v>
+      </c>
+      <c r="M64" t="s">
+        <v>13</v>
+      </c>
+      <c r="N64">
+        <v>353.82</v>
+      </c>
+      <c r="O64">
+        <v>8.8454999999999992E-3</v>
+      </c>
+    </row>
+    <row r="65" spans="12:16" x14ac:dyDescent="0.3">
+      <c r="L65" t="s">
+        <v>20</v>
+      </c>
+      <c r="M65" t="s">
+        <v>14</v>
+      </c>
+      <c r="N65">
+        <v>351.66</v>
+      </c>
+      <c r="O65">
+        <v>7.0331999999999999E-3</v>
+      </c>
+    </row>
+    <row r="66" spans="12:16" x14ac:dyDescent="0.3">
+      <c r="L66" t="s">
+        <v>20</v>
+      </c>
+      <c r="M66" t="s">
+        <v>15</v>
+      </c>
+      <c r="N66">
+        <v>349.82</v>
+      </c>
+      <c r="O66">
+        <v>5.830333E-3</v>
+      </c>
+    </row>
+    <row r="67" spans="12:16" x14ac:dyDescent="0.3">
+      <c r="L67" t="s">
+        <v>20</v>
+      </c>
+      <c r="M67" t="s">
+        <v>16</v>
+      </c>
+      <c r="N67">
+        <v>347.52</v>
+      </c>
+      <c r="O67">
+        <v>4.9645710000000001E-3</v>
+      </c>
+    </row>
+    <row r="69" spans="12:16" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="L69" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="M69" s="8"/>
+      <c r="N69" s="8"/>
+      <c r="O69" s="8"/>
+      <c r="P69" s="8"/>
+    </row>
+    <row r="70" spans="12:16" x14ac:dyDescent="0.3">
+      <c r="L70" s="8"/>
+      <c r="M70" s="8"/>
+      <c r="N70" s="8"/>
+      <c r="O70" s="8"/>
+      <c r="P70" s="8"/>
+    </row>
+    <row r="71" spans="12:16" x14ac:dyDescent="0.3">
+      <c r="L71" s="8"/>
+      <c r="M71" s="8"/>
+      <c r="N71" s="8"/>
+      <c r="O71" s="8"/>
+      <c r="P71" s="8"/>
+    </row>
+    <row r="72" spans="12:16" x14ac:dyDescent="0.3">
+      <c r="L72" s="8"/>
+      <c r="M72" s="8"/>
+      <c r="N72" s="8"/>
+      <c r="O72" s="8"/>
+      <c r="P72" s="8"/>
+    </row>
+    <row r="73" spans="12:16" x14ac:dyDescent="0.3">
+      <c r="L73" s="8"/>
+      <c r="M73" s="8"/>
+      <c r="N73" s="8"/>
+      <c r="O73" s="8"/>
+      <c r="P73" s="8"/>
+    </row>
+    <row r="74" spans="12:16" x14ac:dyDescent="0.3">
+      <c r="L74" s="8"/>
+      <c r="M74" s="8"/>
+      <c r="N74" s="8"/>
+      <c r="O74" s="8"/>
+      <c r="P74" s="8"/>
+    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A24:J43">
-    <sortCondition ref="I24:I43"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="L48:O67">
+    <sortCondition descending="1" ref="O48:O67"/>
   </sortState>
-  <mergeCells count="10">
+  <mergeCells count="11">
+    <mergeCell ref="L69:P74"/>
     <mergeCell ref="L28:L31"/>
     <mergeCell ref="L32:L35"/>
     <mergeCell ref="L36:L39"/>

</xml_diff>